<commit_message>
update and added paper
</commit_message>
<xml_diff>
--- a/Data and ML/Synthetic Data/06_Cancer Types Implementation/Cancers_NCBI search hits.xlsx
+++ b/Data and ML/Synthetic Data/06_Cancer Types Implementation/Cancers_NCBI search hits.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\서연\Research+MATLAB\Summer 2018\2_Data and ML\Synthetic Data\06_Cancer Types Implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karen/Documents/Summer 2018/Cancer Driver Genes/Data and ML/Synthetic Data/06_Cancer Types Implementation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1EF5FB2-7BDC-485F-B12C-124504B2419B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02619A38-8BB6-F248-A68F-83B97EB881EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4170" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="16260" yWindow="8500" windowWidth="28060" windowHeight="15220" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colon" sheetId="3" r:id="rId1"/>
     <sheet name="Pancreatic" sheetId="1" r:id="rId2"/>
     <sheet name="Melanoma" sheetId="4" r:id="rId3"/>
     <sheet name="Breast " sheetId="2" r:id="rId4"/>
+    <sheet name="ALL MERGED (cut from Paper)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="111">
   <si>
     <t>Recent queries in pubmed</t>
   </si>
@@ -266,13 +267,103 @@
   </si>
   <si>
     <t>Search (RHOA) AND melanoma</t>
+  </si>
+  <si>
+    <t>Colorectal Cancer</t>
+  </si>
+  <si>
+    <t>Pancreatic Cancer</t>
+  </si>
+  <si>
+    <t>Breast Cancer</t>
+  </si>
+  <si>
+    <t>Melanoma</t>
+  </si>
+  <si>
+    <t>RHOA</t>
+  </si>
+  <si>
+    <t>KRAS</t>
+  </si>
+  <si>
+    <t>BRAF</t>
+  </si>
+  <si>
+    <t>NFE2L2</t>
+  </si>
+  <si>
+    <t>PIK3CA</t>
+  </si>
+  <si>
+    <t>IDH2</t>
+  </si>
+  <si>
+    <t>CDK4</t>
+  </si>
+  <si>
+    <t>SPOP</t>
+  </si>
+  <si>
+    <t>AKT1</t>
+  </si>
+  <si>
+    <t>U2AF1</t>
+  </si>
+  <si>
+    <t>P2RY8</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>TP53</t>
+  </si>
+  <si>
+    <t>HRAS</t>
+  </si>
+  <si>
+    <t>DNMT3A</t>
+  </si>
+  <si>
+    <t>PTEN</t>
+  </si>
+  <si>
+    <t>FAT4</t>
+  </si>
+  <si>
+    <t>USP8</t>
+  </si>
+  <si>
+    <t>LRP1B</t>
+  </si>
+  <si>
+    <t>MYD88</t>
+  </si>
+  <si>
+    <t>ERBB2</t>
+  </si>
+  <si>
+    <t>PPP6C</t>
+  </si>
+  <si>
+    <t>PTPRT</t>
+  </si>
+  <si>
+    <t>EP300</t>
+  </si>
+  <si>
+    <t>RAC1</t>
+  </si>
+  <si>
+    <t>NCOR1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +498,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -589,7 +686,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -704,6 +801,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -749,9 +946,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1106,25 +1327,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.1796875" defaultRowHeight="20.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="20.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1368,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1380,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1171,7 +1392,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1183,7 +1404,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1416,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1207,7 +1428,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1219,7 +1440,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1231,7 +1452,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1464,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1255,7 +1476,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1267,7 +1488,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1279,7 +1500,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1291,7 +1512,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1524,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1321,24 +1542,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="23.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="23.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1349,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1582,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1373,7 +1594,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1385,7 +1606,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1397,7 +1618,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1409,7 +1630,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1421,7 +1642,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1654,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1445,7 +1666,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1457,7 +1678,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1469,7 +1690,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1481,7 +1702,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1493,7 +1714,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1505,7 +1726,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1517,7 +1738,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1529,7 +1750,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1547,25 +1768,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.7265625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1576,7 +1797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1588,7 +1809,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1600,7 +1821,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1612,7 +1833,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1845,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1636,7 +1857,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1869,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1881,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1672,7 +1893,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1684,7 +1905,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1696,7 +1917,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1929,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1720,7 +1941,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1953,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1744,7 +1965,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1762,25 +1983,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1791,7 +2012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1803,7 +2024,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1815,7 +2036,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1827,7 +2048,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1839,7 +2060,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1851,7 +2072,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1863,7 +2084,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1875,7 +2096,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1887,7 +2108,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1899,7 +2120,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1911,7 +2132,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1923,7 +2144,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1935,7 +2156,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1947,7 +2168,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1959,7 +2180,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1974,4 +2195,433 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AB0747-74D2-8645-8361-1597207F67A3}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3">
+        <v>131</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1582</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="3">
+        <v>383</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="3">
+        <v>995</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="3">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="3">
+        <v>332</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1281</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3">
+        <v>83</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="3">
+        <v>405</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="3">
+        <v>151</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="3">
+        <v>138</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="3">
+        <v>282</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="3">
+        <v>883</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="3">
+        <v>204</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="3">
+        <v>116</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="3">
+        <v>850</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="3">
+        <v>439</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1012</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="3">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3">
+        <v>265</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="3">
+        <v>211</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="3">
+        <v>175</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="3">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="3">
+        <v>71</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="3">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="3">
+        <v>343</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="3">
+        <v>675</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="3">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="3">
+        <v>718</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="3">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="3">
+        <v>56</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="3">
+        <v>363</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>